<commit_message>
Agregar Simulated annealing y tests estadísticos
</commit_message>
<xml_diff>
--- a/Reportes/Reporte_Data_40_Salidas_composición_zonas_heterogéneas.xlsx_grasp.xlsx
+++ b/Reportes/Reporte_Data_40_Salidas_composición_zonas_heterogéneas.xlsx_grasp.xlsx
@@ -135,10 +135,10 @@
     <t>Pedido_39</t>
   </si>
   <si>
+    <t>Pedido_26</t>
+  </si>
+  <si>
     <t>Pedido_32</t>
-  </si>
-  <si>
-    <t>Pedido_26</t>
   </si>
   <si>
     <t>Pedido_30</t>

</xml_diff>

<commit_message>
Reportes actualizados y beam search añadido
</commit_message>
<xml_diff>
--- a/Reportes/Reporte_Data_40_Salidas_composición_zonas_heterogéneas.xlsx_grasp.xlsx
+++ b/Reportes/Reporte_Data_40_Salidas_composición_zonas_heterogéneas.xlsx_grasp.xlsx
@@ -135,10 +135,10 @@
     <t>Pedido_39</t>
   </si>
   <si>
+    <t>Pedido_32</t>
+  </si>
+  <si>
     <t>Pedido_26</t>
-  </si>
-  <si>
-    <t>Pedido_32</t>
   </si>
   <si>
     <t>Pedido_30</t>

</xml_diff>